<commit_message>
include controls to control the timeout interval for the cursor display thing separately
</commit_message>
<xml_diff>
--- a/others/SetBrightnessAfterMakingAllChecksDocumentation.xlsx
+++ b/others/SetBrightnessAfterMakingAllChecksDocumentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\Documents\Personal_Documents\programming\DDAUpdated\others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F292EA2-1371-467E-8FC7-3403F31867CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49499BE-FEFC-491F-872E-2737251E6740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43170" yWindow="-24660" windowWidth="16440" windowHeight="28320" xr2:uid="{8237BE7F-9A37-4B3C-9E43-760E1FD71310}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{8237BE7F-9A37-4B3C-9E43-760E1FD71310}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>IsCursorOnPrimaryDisplay</t>
-  </si>
-  <si>
     <t>isDimmed (screen is already dimmed)</t>
   </si>
   <si>
@@ -72,20 +69,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">T: 
-If CursorTrackerTimer already started:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">ACTION: </t>
+      <t>ACTION</t>
     </r>
     <r>
       <rPr>
@@ -95,8 +79,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>reset the CursorTrackerTimer (cursor is back on the primary display)</t>
-    </r>
+      <t>s are computationally expensive; avoid as much as possible</t>
+    </r>
+  </si>
+  <si>
+    <t>IsCursorOnPrimaryDisplayBool</t>
   </si>
   <si>
     <r>
@@ -144,13 +131,26 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> and Dispose the Timer
+      <t xml:space="preserve"> and Stop / Reset the Timer
  - else (if CursorTrackerTimer &lt; 2 mins), do not dim, (rerun the loop) </t>
     </r>
   </si>
   <si>
     <r>
-      <t>ACTION</t>
+      <t xml:space="preserve">T: 
+If CursorTrackerTimer already started:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">ACTION: </t>
     </r>
     <r>
       <rPr>
@@ -160,7 +160,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>s are computationally expensive; avoid as much as possible</t>
+      <t>reset the CursorTrackerTimer (cursor is back on the primary display). Then check:</t>
     </r>
   </si>
 </sst>
@@ -608,7 +608,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -621,7 +621,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -629,17 +629,17 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C5" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="7"/>
     </row>
@@ -654,27 +654,27 @@
     </row>
     <row r="7" spans="1:4" ht="123" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="135.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>12</v>
@@ -682,7 +682,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>